<commit_message>
Feature of choices to prevent errors
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -59,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -80,11 +80,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -148,7 +143,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,10 +167,10 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -227,7 +222,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>1321607</v>
+        <v>11321607</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>31</v>

</xml_diff>